<commit_message>
updated backlog for end-user part
</commit_message>
<xml_diff>
--- a/3-Backlog-Sprints.xlsx
+++ b/3-Backlog-Sprints.xlsx
@@ -19,35 +19,39 @@
     <definedName function="false" hidden="true" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">'Sprint 1'!$A$6:$E$16</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm.Print_Area" vbProcedure="false">'Sprint 2'!$A$1:$N$16</definedName>
     <definedName function="false" hidden="true" localSheetId="3" name="_xlnm._FilterDatabase" vbProcedure="false">'Sprint 2'!$A$6:$E$17</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">'Product Backlog'!$B$4:$H$119</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0" vbProcedure="false">'Product Backlog'!$B$4:$H$119</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">'Product Backlog'!$B$4:$H$119</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">'Product Backlog'!$B$4:$H$119</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">'Product Backlog'!$B$4:$H$119</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">'Product Backlog'!$B$4:$H$126</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0" vbProcedure="false">'Product Backlog'!$B$4:$H$126</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">'Product Backlog'!$B$4:$H$126</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">'Product Backlog'!$B$4:$H$126</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">'Product Backlog'!$B$4:$H$126</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm.Print_Area" vbProcedure="false">'Sprint 1'!$A$1:$N$15</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm.Print_Area_0" vbProcedure="false">'Sprint 1'!$A$1:$N$15</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm.Print_Area_0_0" vbProcedure="false">'Sprint 1'!$A$1:$N$15</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm.Print_Area_0_0_0" vbProcedure="false">'Sprint 1'!$A$1:$N$15</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm.Print_Area_0_0_0_0" vbProcedure="false">'Sprint 1'!$A$1:$N$15</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm.Print_Area_0_0_0_0_0" vbProcedure="false">'Sprint 1'!$A$1:$N$15</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm.Print_Area_0_0_0_0_0_0" vbProcedure="false">'Sprint 1'!$A$1:$N$15</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">'Sprint 1'!$A$6:$E$16</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0" vbProcedure="false">'Sprint 1'!$A$6:$E$16</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">'Sprint 1'!$A$6:$E$16</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">'Sprint 1'!$A$6:$E$16</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">'Sprint 1'!$A$6:$E$16</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0" vbProcedure="false">'Sprint 1'!$A$6:$E$16</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0_0" vbProcedure="false">'Sprint 1'!$A$6:$E$16</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm.Print_Area" vbProcedure="false">'Sprint 2'!$A$1:$N$16</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm.Print_Area_0" vbProcedure="false">'Sprint 2'!$A$1:$N$16</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm.Print_Area_0_0" vbProcedure="false">'Sprint 2'!$A$1:$N$16</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm.Print_Area_0_0_0" vbProcedure="false">'Sprint 2'!$A$1:$N$16</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm.Print_Area_0_0_0_0" vbProcedure="false">'Sprint 2'!$A$1:$N$16</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm.Print_Area_0_0_0_0_0" vbProcedure="false">'Sprint 2'!$A$1:$N$16</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm.Print_Area_0_0_0_0_0_0" vbProcedure="false">'Sprint 2'!$A$1:$N$16</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase" vbProcedure="false">'Sprint 2'!$A$6:$E$17</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0" vbProcedure="false">'Sprint 2'!$A$6:$E$17</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">'Sprint 2'!$A$6:$E$17</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">'Sprint 2'!$A$6:$E$17</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">'Sprint 2'!$A$6:$E$17</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0" vbProcedure="false">'Sprint 2'!$A$6:$E$17</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0" vbProcedure="false">'Sprint 2'!$A$6:$E$17</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -468,7 +472,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="108">
   <si>
     <t xml:space="preserve">Scrum Excel sheet</t>
   </si>
@@ -623,16 +627,16 @@
     <t xml:space="preserve">Rechercher un trajet</t>
   </si>
   <si>
-    <t xml:space="preserve">Trajet – passager</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Saisir un trajet</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Trajet – conducteur</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Voir le profil public d’un autre utilisateur</t>
+    <t xml:space="preserve">Trajet – réservation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Voir la liste des trajets correspondants à ma recherche</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Voir le détail d’un trajet de la liste de réponse</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Voir le profil public d’un autre utilisateur depuis la page de détail d’un trajet</t>
   </si>
   <si>
     <t xml:space="preserve">Profils</t>
@@ -641,6 +645,9 @@
     <t xml:space="preserve">Utilisateur</t>
   </si>
   <si>
+    <t xml:space="preserve">Voir le profil complet d’un autre utilisateur depuis la page de détail d’un trajet</t>
+  </si>
+  <si>
     <t xml:space="preserve">Modifier mon compte</t>
   </si>
   <si>
@@ -650,49 +657,76 @@
     <t xml:space="preserve">Définir mon ou mes véhicules</t>
   </si>
   <si>
-    <t xml:space="preserve">Voir le profil complet d’un autre utilisateur</t>
+    <t xml:space="preserve">Utilisateur – passager</t>
   </si>
   <si>
     <t xml:space="preserve">Réserver un trajet</t>
   </si>
   <si>
-    <t xml:space="preserve">Annuler une réservation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Valider un trajet</t>
-  </si>
-  <si>
     <t xml:space="preserve">Payer mon trajet</t>
   </si>
   <si>
+    <t xml:space="preserve">Utilisateur – conducteur</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Créer un trajet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Trajet – création</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Voir les trajets en cours</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Trajets en cours</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Voir les réservations passager sur mon trajet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Accepter ou refuser les réservations sur mon trajet</t>
+  </si>
+  <si>
     <t xml:space="preserve">Valider ma présence au point de rendez-vous</t>
   </si>
   <si>
-    <t xml:space="preserve">Trajet – passager et conducteur</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Annuler un trajet</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Voir les réservations passager sur mon trajet</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Accepter ou refuser les réservations sur mon trajet</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Voir les trajets en cours</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Liste trajets</t>
+    <t xml:space="preserve">Modifier un trajet que j’ai créé et qui n’a pas encore de passagers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Modifier un trajet que j’ai créé et qui a déjà des passagers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Annuler ma réservation sur un trajet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Annuler un trajet que j’ai créé</t>
   </si>
   <si>
     <t xml:space="preserve">Voir les trajets effectués</t>
   </si>
   <si>
+    <t xml:space="preserve">Trajets passés</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Voir le détail d’un trajet que j’ai effectué en tant que passager</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Voir le détail d’un trajet que j’ai créé</t>
+  </si>
+  <si>
     <t xml:space="preserve">Evaluer un utilisateur avec qui j’ai partagé un trajet</t>
   </si>
   <si>
-    <t xml:space="preserve">Administrateur</t>
+    <t xml:space="preserve">déclarer qu’un autre utilisateur qui devait faire le trajet avec moi était absent</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Voir la page à propos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A propos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Administrateur ou super admin</t>
   </si>
   <si>
     <t xml:space="preserve">Me connecter au back-office</t>
@@ -708,6 +742,12 @@
   </si>
   <si>
     <t xml:space="preserve">Définir le taux de comission du site</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Super-Admin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gérer les comptes admin</t>
   </si>
   <si>
     <t xml:space="preserve">Sprint 1</t>
@@ -1824,7 +1864,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1871,8 +1911,8 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.359157578036856"/>
-          <c:y val="0.0436507936507936"/>
+          <c:x val="0.359171085787356"/>
+          <c:y val="0.0436552355754554"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -1884,10 +1924,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.102895825498308"/>
-          <c:y val="0.203805453805454"/>
-          <c:w val="0.721286197818729"/>
-          <c:h val="0.59015059015059"/>
+          <c:x val="0.102899695362744"/>
+          <c:y val="0.203826193141345"/>
+          <c:w val="0.721275715521456"/>
+          <c:h val="0.590108883687799"/>
         </c:manualLayout>
       </c:layout>
       <c:lineChart>
@@ -2069,11 +2109,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="1"/>
-        <c:axId val="45426305"/>
-        <c:axId val="66863910"/>
+        <c:axId val="67282837"/>
+        <c:axId val="95339777"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="45426305"/>
+        <c:axId val="67282837"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2121,8 +2161,8 @@
             <c:manualLayout>
               <c:xMode val="edge"/>
               <c:yMode val="edge"/>
-              <c:x val="0.435276419706657"/>
-              <c:y val="0.885632885632886"/>
+              <c:x val="0.435292790251608"/>
+              <c:y val="0.885621247583189"/>
             </c:manualLayout>
           </c:layout>
           <c:overlay val="0"/>
@@ -2158,14 +2198,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="66863910"/>
+        <c:crossAx val="95339777"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="66863910"/>
+        <c:axId val="95339777"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2213,8 +2253,8 @@
             <c:manualLayout>
               <c:xMode val="edge"/>
               <c:yMode val="edge"/>
-              <c:x val="0.0302369311771343"/>
-              <c:y val="0.361416361416361"/>
+              <c:x val="0.0302756779119185"/>
+              <c:y val="0.361351378854177"/>
             </c:manualLayout>
           </c:layout>
           <c:overlay val="0"/>
@@ -2250,7 +2290,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="45426305"/>
+        <c:crossAx val="67282837"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2314,7 +2354,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -2361,8 +2401,8 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.359188896544935"/>
-          <c:y val="0.0436552355754554"/>
+          <c:x val="0.359206575773982"/>
+          <c:y val="0.0436596784042337"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -2374,10 +2414,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.102913672605571"/>
-          <c:y val="0.203826193141345"/>
-          <c:w val="0.721232404764248"/>
-          <c:h val="0.590210644143686"/>
+          <c:x val="0.102918738002658"/>
+          <c:y val="0.203846936698555"/>
+          <c:w val="0.721218683860806"/>
+          <c:h val="0.590168939548138"/>
         </c:manualLayout>
       </c:layout>
       <c:lineChart>
@@ -2559,11 +2599,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="1"/>
-        <c:axId val="96612351"/>
-        <c:axId val="79736778"/>
+        <c:axId val="68327652"/>
+        <c:axId val="83634385"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="96612351"/>
+        <c:axId val="68327652"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2611,8 +2651,8 @@
             <c:manualLayout>
               <c:xMode val="edge"/>
               <c:yMode val="edge"/>
-              <c:x val="0.435328280342553"/>
-              <c:y val="0.885621247583189"/>
+              <c:x val="0.435349707141802"/>
+              <c:y val="0.885609607164665"/>
             </c:manualLayout>
           </c:layout>
           <c:overlay val="0"/>
@@ -2648,14 +2688,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="79736778"/>
+        <c:crossAx val="83634385"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="79736778"/>
+        <c:axId val="83634385"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2703,8 +2743,8 @@
             <c:manualLayout>
               <c:xMode val="edge"/>
               <c:yMode val="edge"/>
-              <c:x val="0.0303179446795944"/>
-              <c:y val="0.361351378854177"/>
+              <c:x val="0.0303686567898804"/>
+              <c:y val="0.361184612253206"/>
             </c:manualLayout>
           </c:layout>
           <c:overlay val="0"/>
@@ -2740,7 +2780,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="96612351"/>
+        <c:crossAx val="68327652"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2815,9 +2855,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>615240</xdr:colOff>
+      <xdr:colOff>614880</xdr:colOff>
       <xdr:row>36</xdr:row>
-      <xdr:rowOff>158040</xdr:rowOff>
+      <xdr:rowOff>157680</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2831,7 +2871,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="533520" y="6004440"/>
-          <a:ext cx="832680" cy="297000"/>
+          <a:ext cx="832320" cy="296640"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2857,9 +2897,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>455040</xdr:colOff>
+      <xdr:colOff>454680</xdr:colOff>
       <xdr:row>46</xdr:row>
-      <xdr:rowOff>155160</xdr:rowOff>
+      <xdr:rowOff>154800</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2868,7 +2908,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="640080" y="4293720"/>
-        <a:ext cx="9572040" cy="3537720"/>
+        <a:ext cx="9571680" cy="3537360"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2892,9 +2932,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>455040</xdr:colOff>
+      <xdr:colOff>454680</xdr:colOff>
       <xdr:row>40</xdr:row>
-      <xdr:rowOff>135360</xdr:rowOff>
+      <xdr:rowOff>135000</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2903,7 +2943,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="640080" y="4255920"/>
-        <a:ext cx="7314120" cy="3537360"/>
+        <a:ext cx="7313760" cy="3537000"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -3745,10 +3785,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I34"/>
+  <dimension ref="A1:I41"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E21" activeCellId="0" sqref="E21"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B10" colorId="64" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C38" activeCellId="0" sqref="C38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3905,7 +3945,7 @@
         <v>40</v>
       </c>
       <c r="E10" s="29" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="F10" s="29"/>
       <c r="G10" s="29"/>
@@ -3914,13 +3954,13 @@
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="29"/>
       <c r="C11" s="29" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="D11" s="29" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E11" s="29" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="F11" s="29"/>
       <c r="G11" s="29"/>
@@ -3929,13 +3969,13 @@
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="29"/>
       <c r="C12" s="29" t="s">
-        <v>44</v>
+        <v>30</v>
       </c>
       <c r="D12" s="29" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="E12" s="29" t="s">
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="F12" s="29"/>
       <c r="G12" s="29"/>
@@ -3947,10 +3987,10 @@
         <v>44</v>
       </c>
       <c r="D13" s="29" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E13" s="29" t="s">
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="F13" s="29"/>
       <c r="G13" s="29"/>
@@ -3962,7 +4002,7 @@
         <v>44</v>
       </c>
       <c r="D14" s="29" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E14" s="29" t="s">
         <v>34</v>
@@ -3977,10 +4017,10 @@
         <v>44</v>
       </c>
       <c r="D15" s="29" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E15" s="29" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
       <c r="F15" s="29"/>
       <c r="G15" s="29"/>
@@ -3992,10 +4032,10 @@
         <v>44</v>
       </c>
       <c r="D16" s="29" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E16" s="29" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="F16" s="29"/>
       <c r="G16" s="29"/>
@@ -4004,7 +4044,7 @@
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B17" s="29"/>
       <c r="C17" s="29" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="D17" s="29" t="s">
         <v>50</v>
@@ -4019,13 +4059,13 @@
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B18" s="29"/>
       <c r="C18" s="29" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="D18" s="29" t="s">
         <v>51</v>
       </c>
       <c r="E18" s="29" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="F18" s="29"/>
       <c r="G18" s="29"/>
@@ -4034,28 +4074,28 @@
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B19" s="29"/>
       <c r="C19" s="29" t="s">
-        <v>44</v>
+        <v>52</v>
       </c>
       <c r="D19" s="29" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="E19" s="29" t="s">
-        <v>39</v>
+        <v>54</v>
       </c>
       <c r="F19" s="29"/>
       <c r="G19" s="29"/>
       <c r="H19" s="29"/>
     </row>
-    <row r="20" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B20" s="29"/>
       <c r="C20" s="29" t="s">
         <v>44</v>
       </c>
       <c r="D20" s="29" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="E20" s="29" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="F20" s="29"/>
       <c r="G20" s="29"/>
@@ -4064,13 +4104,13 @@
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B21" s="29"/>
       <c r="C21" s="29" t="s">
-        <v>44</v>
+        <v>52</v>
       </c>
       <c r="D21" s="29" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E21" s="29" t="s">
-        <v>41</v>
+        <v>56</v>
       </c>
       <c r="F21" s="29"/>
       <c r="G21" s="29"/>
@@ -4079,13 +4119,13 @@
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B22" s="29"/>
       <c r="C22" s="29" t="s">
-        <v>44</v>
+        <v>52</v>
       </c>
       <c r="D22" s="29" t="s">
+        <v>58</v>
+      </c>
+      <c r="E22" s="29" t="s">
         <v>56</v>
-      </c>
-      <c r="E22" s="29" t="s">
-        <v>41</v>
       </c>
       <c r="F22" s="29"/>
       <c r="G22" s="29"/>
@@ -4097,10 +4137,10 @@
         <v>44</v>
       </c>
       <c r="D23" s="29" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="E23" s="29" t="s">
-        <v>41</v>
+        <v>56</v>
       </c>
       <c r="F23" s="29"/>
       <c r="G23" s="29"/>
@@ -4109,13 +4149,13 @@
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B24" s="29"/>
       <c r="C24" s="29" t="s">
-        <v>44</v>
+        <v>52</v>
       </c>
       <c r="D24" s="29" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="E24" s="29" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="F24" s="29"/>
       <c r="G24" s="29"/>
@@ -4124,13 +4164,13 @@
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B25" s="29"/>
       <c r="C25" s="29" t="s">
-        <v>44</v>
+        <v>52</v>
       </c>
       <c r="D25" s="29" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="E25" s="29" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="F25" s="29"/>
       <c r="G25" s="29"/>
@@ -4139,13 +4179,13 @@
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B26" s="29"/>
       <c r="C26" s="29" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="D26" s="29" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="E26" s="29" t="s">
-        <v>43</v>
+        <v>56</v>
       </c>
       <c r="F26" s="29"/>
       <c r="G26" s="29"/>
@@ -4154,13 +4194,13 @@
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B27" s="29"/>
       <c r="C27" s="29" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
       <c r="D27" s="29" t="s">
         <v>63</v>
       </c>
       <c r="E27" s="29" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="F27" s="29"/>
       <c r="G27" s="29"/>
@@ -4169,13 +4209,13 @@
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B28" s="29"/>
       <c r="C28" s="29" t="s">
-        <v>62</v>
+        <v>44</v>
       </c>
       <c r="D28" s="29" t="s">
+        <v>64</v>
+      </c>
+      <c r="E28" s="29" t="s">
         <v>65</v>
-      </c>
-      <c r="E28" s="29" t="s">
-        <v>64</v>
       </c>
       <c r="F28" s="29"/>
       <c r="G28" s="29"/>
@@ -4184,13 +4224,13 @@
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B29" s="29"/>
       <c r="C29" s="29" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
       <c r="D29" s="29" t="s">
         <v>66</v>
       </c>
       <c r="E29" s="29" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="F29" s="29"/>
       <c r="G29" s="29"/>
@@ -4199,13 +4239,13 @@
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B30" s="29"/>
       <c r="C30" s="29" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
       <c r="D30" s="29" t="s">
         <v>67</v>
       </c>
       <c r="E30" s="29" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="F30" s="29"/>
       <c r="G30" s="29"/>
@@ -4213,39 +4253,150 @@
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B31" s="29"/>
-      <c r="C31" s="29"/>
-      <c r="D31" s="29"/>
-      <c r="E31" s="29"/>
+      <c r="C31" s="29" t="s">
+        <v>44</v>
+      </c>
+      <c r="D31" s="29" t="s">
+        <v>68</v>
+      </c>
+      <c r="E31" s="29" t="s">
+        <v>65</v>
+      </c>
       <c r="F31" s="29"/>
       <c r="G31" s="29"/>
       <c r="H31" s="29"/>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B32" s="29"/>
-      <c r="C32" s="29"/>
-      <c r="D32" s="29"/>
-      <c r="E32" s="29"/>
+      <c r="C32" s="29" t="s">
+        <v>44</v>
+      </c>
+      <c r="D32" s="29" t="s">
+        <v>69</v>
+      </c>
+      <c r="E32" s="29" t="s">
+        <v>65</v>
+      </c>
       <c r="F32" s="29"/>
       <c r="G32" s="29"/>
       <c r="H32" s="29"/>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B33" s="29"/>
-      <c r="C33" s="29"/>
-      <c r="D33" s="29"/>
-      <c r="E33" s="29"/>
+      <c r="C33" s="29" t="s">
+        <v>44</v>
+      </c>
+      <c r="D33" s="29" t="s">
+        <v>70</v>
+      </c>
+      <c r="E33" s="29" t="s">
+        <v>71</v>
+      </c>
       <c r="F33" s="29"/>
       <c r="G33" s="29"/>
       <c r="H33" s="29"/>
     </row>
-    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B34" s="31"/>
-      <c r="C34" s="31"/>
-      <c r="D34" s="31"/>
-      <c r="E34" s="31"/>
-      <c r="F34" s="31"/>
-      <c r="G34" s="31"/>
-      <c r="H34" s="31"/>
+    <row r="34" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B34" s="29"/>
+      <c r="C34" s="29" t="s">
+        <v>72</v>
+      </c>
+      <c r="D34" s="29" t="s">
+        <v>73</v>
+      </c>
+      <c r="E34" s="29" t="s">
+        <v>74</v>
+      </c>
+      <c r="F34" s="29"/>
+      <c r="G34" s="29"/>
+      <c r="H34" s="29"/>
+    </row>
+    <row r="35" customFormat="false" ht="17.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B35" s="29"/>
+      <c r="C35" s="29" t="s">
+        <v>72</v>
+      </c>
+      <c r="D35" s="29" t="s">
+        <v>75</v>
+      </c>
+      <c r="E35" s="29" t="s">
+        <v>74</v>
+      </c>
+      <c r="F35" s="29"/>
+      <c r="G35" s="29"/>
+      <c r="H35" s="29"/>
+    </row>
+    <row r="36" customFormat="false" ht="17.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B36" s="29"/>
+      <c r="C36" s="29" t="s">
+        <v>72</v>
+      </c>
+      <c r="D36" s="29" t="s">
+        <v>76</v>
+      </c>
+      <c r="E36" s="29" t="s">
+        <v>74</v>
+      </c>
+      <c r="F36" s="29"/>
+      <c r="G36" s="29"/>
+      <c r="H36" s="29"/>
+    </row>
+    <row r="37" customFormat="false" ht="17.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B37" s="29"/>
+      <c r="C37" s="29" t="s">
+        <v>72</v>
+      </c>
+      <c r="D37" s="29" t="s">
+        <v>77</v>
+      </c>
+      <c r="E37" s="29" t="s">
+        <v>74</v>
+      </c>
+      <c r="F37" s="29"/>
+      <c r="G37" s="29"/>
+      <c r="H37" s="29"/>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B38" s="29"/>
+      <c r="C38" s="29" t="s">
+        <v>78</v>
+      </c>
+      <c r="D38" s="29" t="s">
+        <v>79</v>
+      </c>
+      <c r="E38" s="29" t="s">
+        <v>74</v>
+      </c>
+      <c r="F38" s="29"/>
+      <c r="G38" s="29"/>
+      <c r="H38" s="29"/>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B39" s="29"/>
+      <c r="C39" s="29"/>
+      <c r="D39" s="29"/>
+      <c r="E39" s="29"/>
+      <c r="F39" s="29"/>
+      <c r="G39" s="29"/>
+      <c r="H39" s="29"/>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B40" s="29"/>
+      <c r="C40" s="29"/>
+      <c r="D40" s="29"/>
+      <c r="E40" s="29"/>
+      <c r="F40" s="29"/>
+      <c r="G40" s="29"/>
+      <c r="H40" s="29"/>
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B41" s="31"/>
+      <c r="C41" s="31"/>
+      <c r="D41" s="31"/>
+      <c r="E41" s="31"/>
+      <c r="F41" s="31"/>
+      <c r="G41" s="31"/>
+      <c r="H41" s="31"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -4286,10 +4437,10 @@
     <row r="1" customFormat="false" ht="20.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1"/>
       <c r="B1" s="32" t="s">
-        <v>68</v>
+        <v>80</v>
       </c>
       <c r="C1" s="33" t="s">
-        <v>69</v>
+        <v>81</v>
       </c>
       <c r="D1" s="34" t="n">
         <v>39742</v>
@@ -4313,7 +4464,7 @@
         <v>My Product</v>
       </c>
       <c r="C2" s="33" t="s">
-        <v>70</v>
+        <v>82</v>
       </c>
       <c r="D2" s="34" t="n">
         <f aca="false">WORKDAY(D1,10)</f>
@@ -4346,7 +4497,7 @@
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="33" t="s">
-        <v>71</v>
+        <v>83</v>
       </c>
       <c r="D3" s="38" t="n">
         <f aca="false">D16</f>
@@ -4379,10 +4530,10 @@
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="33" t="s">
-        <v>72</v>
+        <v>84</v>
       </c>
       <c r="D4" s="39" t="s">
-        <v>73</v>
+        <v>85</v>
       </c>
       <c r="E4" s="39"/>
       <c r="F4" s="39"/>
@@ -4437,16 +4588,16 @@
     </row>
     <row r="6" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="40" t="s">
-        <v>74</v>
+        <v>86</v>
       </c>
       <c r="B6" s="41" t="s">
-        <v>75</v>
+        <v>87</v>
       </c>
       <c r="C6" s="42" t="s">
-        <v>76</v>
+        <v>88</v>
       </c>
       <c r="D6" s="43" t="s">
-        <v>77</v>
+        <v>89</v>
       </c>
       <c r="E6" s="44" t="n">
         <v>39650</v>
@@ -4770,7 +4921,7 @@
         <v>0</v>
       </c>
       <c r="O16" s="73" t="s">
-        <v>78</v>
+        <v>90</v>
       </c>
       <c r="P16" s="37"/>
       <c r="Q16" s="37"/>
@@ -4855,7 +5006,7 @@
       <c r="B17" s="70"/>
       <c r="C17" s="37"/>
       <c r="D17" s="74" t="s">
-        <v>79</v>
+        <v>91</v>
       </c>
       <c r="E17" s="75" t="n">
         <f aca="false">'system sheet'!C10</f>
@@ -7448,10 +7599,10 @@
     <row r="1" customFormat="false" ht="53.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="1"/>
       <c r="B1" s="32" t="s">
-        <v>80</v>
+        <v>92</v>
       </c>
       <c r="C1" s="33" t="s">
-        <v>69</v>
+        <v>81</v>
       </c>
       <c r="D1" s="34" t="n">
         <v>39742</v>
@@ -7474,7 +7625,7 @@
         <v>My Product</v>
       </c>
       <c r="C2" s="33" t="s">
-        <v>70</v>
+        <v>82</v>
       </c>
       <c r="D2" s="34" t="n">
         <f aca="false">WORKDAY(D1,10)</f>
@@ -7507,7 +7658,7 @@
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="33" t="s">
-        <v>71</v>
+        <v>83</v>
       </c>
       <c r="D3" s="38" t="n">
         <f aca="false">D17</f>
@@ -7540,10 +7691,10 @@
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="33" t="s">
-        <v>72</v>
+        <v>84</v>
       </c>
       <c r="D4" s="39" t="s">
-        <v>73</v>
+        <v>85</v>
       </c>
       <c r="E4" s="39"/>
       <c r="F4" s="39"/>
@@ -7598,16 +7749,16 @@
     </row>
     <row r="6" customFormat="false" ht="32.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="40" t="s">
-        <v>81</v>
+        <v>93</v>
       </c>
       <c r="B6" s="41" t="s">
-        <v>82</v>
+        <v>94</v>
       </c>
       <c r="C6" s="42" t="s">
-        <v>76</v>
+        <v>88</v>
       </c>
       <c r="D6" s="43" t="s">
-        <v>77</v>
+        <v>89</v>
       </c>
       <c r="E6" s="44" t="n">
         <v>39650</v>
@@ -7721,7 +7872,7 @@
     <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="86"/>
       <c r="B7" s="48" t="s">
-        <v>83</v>
+        <v>95</v>
       </c>
       <c r="C7" s="49"/>
       <c r="D7" s="50" t="n">
@@ -7945,7 +8096,7 @@
         <v>0</v>
       </c>
       <c r="O17" s="88" t="s">
-        <v>78</v>
+        <v>90</v>
       </c>
       <c r="P17" s="37"/>
       <c r="Q17" s="37"/>
@@ -8030,7 +8181,7 @@
       <c r="B18" s="70"/>
       <c r="C18" s="37"/>
       <c r="D18" s="74" t="s">
-        <v>79</v>
+        <v>91</v>
       </c>
       <c r="E18" s="75" t="n">
         <f aca="false">'system sheet'!C11</f>
@@ -8193,7 +8344,7 @@
     <row r="1" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="2" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="90" t="s">
-        <v>84</v>
+        <v>96</v>
       </c>
       <c r="C2" s="90"/>
       <c r="D2" s="90"/>
@@ -8211,27 +8362,27 @@
     </row>
     <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C5" s="92" t="s">
-        <v>68</v>
+        <v>80</v>
       </c>
       <c r="D5" s="92" t="s">
-        <v>80</v>
+        <v>92</v>
       </c>
       <c r="E5" s="92" t="s">
-        <v>85</v>
+        <v>97</v>
       </c>
       <c r="F5" s="92" t="s">
-        <v>86</v>
+        <v>98</v>
       </c>
       <c r="G5" s="92" t="s">
-        <v>87</v>
+        <v>99</v>
       </c>
       <c r="H5" s="92" t="s">
-        <v>88</v>
+        <v>100</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="93" t="s">
-        <v>89</v>
+        <v>101</v>
       </c>
       <c r="B6" s="93"/>
       <c r="C6" s="94" t="n">
@@ -8247,7 +8398,7 @@
     </row>
     <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="6" t="s">
-        <v>90</v>
+        <v>102</v>
       </c>
       <c r="C7" s="97" t="n">
         <v>0</v>
@@ -8273,10 +8424,10 @@
     </row>
     <row r="9" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="99" t="s">
-        <v>91</v>
+        <v>103</v>
       </c>
       <c r="B9" s="100" t="s">
-        <v>92</v>
+        <v>104</v>
       </c>
       <c r="C9" s="101" t="n">
         <v>0</v>
@@ -8309,13 +8460,13 @@
         <v>9</v>
       </c>
       <c r="N9" s="103" t="s">
-        <v>93</v>
+        <v>105</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="99"/>
       <c r="B10" s="104" t="s">
-        <v>68</v>
+        <v>80</v>
       </c>
       <c r="C10" s="105" t="n">
         <f aca="false">FORECAST(C$9, $C$6:$C$7,$N$10:$N$11)</f>
@@ -8364,7 +8515,7 @@
     <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="99"/>
       <c r="B11" s="104" t="s">
-        <v>80</v>
+        <v>92</v>
       </c>
       <c r="C11" s="105" t="n">
         <f aca="false">FORECAST(C$9, $D$6:$D$7,$N$10:$N$11)</f>
@@ -8413,7 +8564,7 @@
     <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="99"/>
       <c r="B12" s="104" t="s">
-        <v>85</v>
+        <v>97</v>
       </c>
       <c r="C12" s="105"/>
       <c r="D12" s="105"/>
@@ -8432,7 +8583,7 @@
     <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="99"/>
       <c r="B13" s="104" t="s">
-        <v>86</v>
+        <v>98</v>
       </c>
       <c r="C13" s="105"/>
       <c r="D13" s="105"/>
@@ -8448,7 +8599,7 @@
     <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="99"/>
       <c r="B14" s="104" t="s">
-        <v>87</v>
+        <v>99</v>
       </c>
       <c r="C14" s="105"/>
       <c r="D14" s="105"/>
@@ -8464,7 +8615,7 @@
     <row r="15" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="99"/>
       <c r="B15" s="104" t="s">
-        <v>88</v>
+        <v>100</v>
       </c>
       <c r="C15" s="105"/>
       <c r="D15" s="105"/>
@@ -8591,12 +8742,12 @@
     </row>
     <row r="28" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B28" s="5" t="s">
-        <v>94</v>
+        <v>106</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B29" s="6" t="s">
-        <v>95</v>
+        <v>107</v>
       </c>
     </row>
   </sheetData>

</xml_diff>